<commit_message>
Add QA database credentials and import FromlotModule***
***Update imports in app.module.ts***

***Add Post method in database.controller.ts***

***Add axios and https imports in database.service.ts***

***Update work.xlsx
</commit_message>
<xml_diff>
--- a/work.xlsx
+++ b/work.xlsx
@@ -2,13 +2,13 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/akilandananjayan/Downloads/SFCS-script/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BAB55B4-BDD6-DA40-8DC2-8D27B3E7CF1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A024EE87-E2AB-6343-B791-236278902801}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13380" yWindow="4560" windowWidth="14400" windowHeight="9660" xr2:uid="{3F6F255D-65E2-FF43-84FC-DFE1205EBB79}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="16">
   <si>
     <t>Item</t>
   </si>
@@ -83,10 +83,31 @@
     <t>C-TEX Width</t>
   </si>
   <si>
-    <t>FWFT00049 00101</t>
-  </si>
-  <si>
-    <t>B</t>
+    <t>FWFT00039 00001</t>
+  </si>
+  <si>
+    <t>W2308120178-01</t>
+  </si>
+  <si>
+    <t>CX</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>W2306220352-01</t>
+  </si>
+  <si>
+    <t>CU</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
   </si>
 </sst>
 </file>
@@ -489,7 +510,7 @@
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:G14"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -528,22 +549,22 @@
         <v>7</v>
       </c>
       <c r="B2">
-        <v>24011100621</v>
-      </c>
-      <c r="C2">
-        <v>24011100621</v>
+        <v>2308120178</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="1">
         <v>9</v>
       </c>
+      <c r="E2">
+        <v>6</v>
+      </c>
       <c r="F2">
-        <v>33</v>
+        <v>72.319999999999993</v>
       </c>
       <c r="G2">
-        <v>152</v>
+        <v>180</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -551,22 +572,22 @@
         <v>7</v>
       </c>
       <c r="B3">
-        <v>24011100621</v>
-      </c>
-      <c r="C3">
-        <v>24011100621</v>
+        <v>2308120178</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="1">
-        <v>1</v>
+        <v>9</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="F3">
-        <v>50.3</v>
+        <v>65.27</v>
       </c>
       <c r="G3">
-        <v>152</v>
+        <v>180</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -574,22 +595,22 @@
         <v>7</v>
       </c>
       <c r="B4">
-        <v>24011100621</v>
-      </c>
-      <c r="C4">
-        <v>24011100621</v>
+        <v>2306220352</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
       </c>
       <c r="D4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="1">
-        <v>16</v>
+        <v>12</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="F4">
-        <v>41.2</v>
+        <v>35.81</v>
       </c>
       <c r="G4">
-        <v>152</v>
+        <v>167</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -597,22 +618,22 @@
         <v>7</v>
       </c>
       <c r="B5">
-        <v>24011100621</v>
-      </c>
-      <c r="C5">
-        <v>24011100621</v>
+        <v>2306220352</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
       </c>
       <c r="D5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" s="1">
-        <v>2</v>
+        <v>12</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="F5">
-        <v>52.2</v>
+        <v>36.24</v>
       </c>
       <c r="G5">
-        <v>152</v>
+        <v>170</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -620,207 +641,47 @@
         <v>7</v>
       </c>
       <c r="B6">
-        <v>24011100621</v>
-      </c>
-      <c r="C6">
-        <v>24011100621</v>
+        <v>2306220352</v>
+      </c>
+      <c r="C6" t="s">
+        <v>11</v>
       </c>
       <c r="D6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" s="1">
-        <v>14</v>
+        <v>12</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="F6">
-        <v>40.299999999999997</v>
+        <v>37.58</v>
       </c>
       <c r="G6">
-        <v>152</v>
+        <v>172</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7">
-        <v>24011100621</v>
-      </c>
-      <c r="C7">
-        <v>24011100621</v>
-      </c>
-      <c r="D7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" s="1">
-        <v>3</v>
-      </c>
-      <c r="F7">
-        <v>27.5</v>
-      </c>
-      <c r="G7">
-        <v>152</v>
-      </c>
+      <c r="E7" s="1"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8">
-        <v>24011100621</v>
-      </c>
-      <c r="C8">
-        <v>24011100621</v>
-      </c>
-      <c r="D8" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" s="1">
-        <v>19</v>
-      </c>
-      <c r="F8">
-        <v>43.7</v>
-      </c>
-      <c r="G8">
-        <v>152</v>
-      </c>
+      <c r="E8" s="1"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9">
-        <v>24011100621</v>
-      </c>
-      <c r="C9">
-        <v>24011100621</v>
-      </c>
-      <c r="D9" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" s="1">
-        <v>21</v>
-      </c>
-      <c r="F9">
-        <v>16.5</v>
-      </c>
-      <c r="G9">
-        <v>152</v>
-      </c>
+      <c r="E9" s="1"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10">
-        <v>24011100621</v>
-      </c>
-      <c r="C10">
-        <v>24011100621</v>
-      </c>
-      <c r="D10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E10" s="1">
-        <v>20</v>
-      </c>
-      <c r="F10">
-        <v>38.4</v>
-      </c>
-      <c r="G10">
-        <v>152</v>
-      </c>
+      <c r="E10" s="1"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11">
-        <v>24011100621</v>
-      </c>
-      <c r="C11">
-        <v>24011100621</v>
-      </c>
-      <c r="D11" t="s">
-        <v>8</v>
-      </c>
-      <c r="E11" s="1">
-        <v>11</v>
-      </c>
-      <c r="F11">
-        <v>42.6</v>
-      </c>
-      <c r="G11">
-        <v>152</v>
-      </c>
+      <c r="E11" s="1"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>7</v>
-      </c>
-      <c r="B12">
-        <v>24011100621</v>
-      </c>
-      <c r="C12">
-        <v>24011100621</v>
-      </c>
-      <c r="D12" t="s">
-        <v>8</v>
-      </c>
-      <c r="E12" s="1">
-        <v>4</v>
-      </c>
-      <c r="F12">
-        <v>28.4</v>
-      </c>
-      <c r="G12">
-        <v>152</v>
-      </c>
+      <c r="E12" s="1"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>7</v>
-      </c>
-      <c r="B13">
-        <v>24011100621</v>
-      </c>
-      <c r="C13">
-        <v>24011100621</v>
-      </c>
-      <c r="D13" t="s">
-        <v>8</v>
-      </c>
-      <c r="E13" s="1">
-        <v>15</v>
-      </c>
-      <c r="F13">
-        <v>36.6</v>
-      </c>
-      <c r="G13">
-        <v>152</v>
-      </c>
+      <c r="E13" s="1"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>7</v>
-      </c>
-      <c r="B14">
-        <v>24011100621</v>
-      </c>
-      <c r="C14">
-        <v>24011100621</v>
-      </c>
-      <c r="D14" t="s">
-        <v>8</v>
-      </c>
-      <c r="E14" s="1">
-        <v>5</v>
-      </c>
-      <c r="F14">
-        <v>30.2</v>
-      </c>
-      <c r="G14">
-        <v>152</v>
-      </c>
+      <c r="E14" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update database credentials and dependencies
</commit_message>
<xml_diff>
--- a/work.xlsx
+++ b/work.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/akilandananjayan/Downloads/SFCS-script/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A024EE87-E2AB-6343-B791-236278902801}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FAC1C86-FAD3-7148-8E37-754B47493CD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13380" yWindow="4560" windowWidth="14400" windowHeight="9660" xr2:uid="{3F6F255D-65E2-FF43-84FC-DFE1205EBB79}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="17">
   <si>
     <t>Item</t>
   </si>
@@ -83,31 +83,34 @@
     <t>C-TEX Width</t>
   </si>
   <si>
-    <t>FWFT00039 00001</t>
-  </si>
-  <si>
-    <t>W2308120178-01</t>
-  </si>
-  <si>
-    <t>CX</t>
-  </si>
-  <si>
-    <t>16</t>
-  </si>
-  <si>
-    <t>W2306220352-01</t>
-  </si>
-  <si>
-    <t>CU</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>3</t>
+    <t>FWFT00073 00006</t>
+  </si>
+  <si>
+    <t>W2305300406-01</t>
+  </si>
+  <si>
+    <t>HK</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>W2305300405-01</t>
+  </si>
+  <si>
+    <t>5E</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>W2305300410-01</t>
+  </si>
+  <si>
+    <t>5B</t>
+  </si>
+  <si>
+    <t>9</t>
   </si>
 </sst>
 </file>
@@ -150,9 +153,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -160,6 +168,7 @@
   <dxfs count="1">
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -510,7 +519,7 @@
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -519,6 +528,7 @@
     <col min="2" max="2" width="13.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
@@ -549,7 +559,7 @@
         <v>7</v>
       </c>
       <c r="B2">
-        <v>2308120178</v>
+        <v>2305300406</v>
       </c>
       <c r="C2" t="s">
         <v>8</v>
@@ -557,14 +567,14 @@
       <c r="D2" t="s">
         <v>9</v>
       </c>
-      <c r="E2">
-        <v>6</v>
+      <c r="E2" s="2">
+        <v>3</v>
       </c>
       <c r="F2">
-        <v>72.319999999999993</v>
+        <v>82.11</v>
       </c>
       <c r="G2">
-        <v>180</v>
+        <v>159</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -572,7 +582,7 @@
         <v>7</v>
       </c>
       <c r="B3">
-        <v>2308120178</v>
+        <v>2305300406</v>
       </c>
       <c r="C3" t="s">
         <v>8</v>
@@ -584,10 +594,10 @@
         <v>10</v>
       </c>
       <c r="F3">
-        <v>65.27</v>
+        <v>71.569999999999993</v>
       </c>
       <c r="G3">
-        <v>180</v>
+        <v>159</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -595,22 +605,22 @@
         <v>7</v>
       </c>
       <c r="B4">
-        <v>2306220352</v>
+        <v>2305300405</v>
       </c>
       <c r="C4" t="s">
         <v>11</v>
       </c>
       <c r="D4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="F4">
-        <v>35.81</v>
+        <v>12.22</v>
       </c>
       <c r="G4">
-        <v>167</v>
+        <v>158</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -618,22 +628,22 @@
         <v>7</v>
       </c>
       <c r="B5">
-        <v>2306220352</v>
+        <v>2305300405</v>
       </c>
       <c r="C5" t="s">
         <v>11</v>
       </c>
       <c r="D5" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F5">
-        <v>36.24</v>
+        <v>84.16</v>
       </c>
       <c r="G5">
-        <v>170</v>
+        <v>158</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -641,26 +651,46 @@
         <v>7</v>
       </c>
       <c r="B6">
-        <v>2306220352</v>
+        <v>2305300410</v>
       </c>
       <c r="C6" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>15</v>
       </c>
       <c r="F6">
-        <v>37.58</v>
+        <v>12.6</v>
       </c>
       <c r="G6">
-        <v>172</v>
+        <v>158</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="E7" s="1"/>
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7">
+        <v>2305300410</v>
+      </c>
+      <c r="C7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7">
+        <v>63.64</v>
+      </c>
+      <c r="G7">
+        <v>169</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="E8" s="1"/>

</xml_diff>

<commit_message>
Refactor imports and remove commented code in app.module.ts, fromlot.controller.ts, and fromlot.service.ts
</commit_message>
<xml_diff>
--- a/work.xlsx
+++ b/work.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/akilandananjayan/Downloads/SFCS-script/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FAC1C86-FAD3-7148-8E37-754B47493CD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{262E95EF-2346-9A40-95C7-D1EDD11842F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13380" yWindow="4560" windowWidth="14400" windowHeight="9660" xr2:uid="{3F6F255D-65E2-FF43-84FC-DFE1205EBB79}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="27">
   <si>
     <t>Item</t>
   </si>
@@ -83,34 +83,64 @@
     <t>C-TEX Width</t>
   </si>
   <si>
-    <t>FWFT00073 00006</t>
-  </si>
-  <si>
-    <t>W2305300406-01</t>
-  </si>
-  <si>
-    <t>HK</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>W2305300405-01</t>
-  </si>
-  <si>
-    <t>5E</t>
+    <t>FWFT00050 00002</t>
+  </si>
+  <si>
+    <t>2309151196</t>
+  </si>
+  <si>
+    <t>CV</t>
+  </si>
+  <si>
+    <t>20B</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>23</t>
   </si>
   <si>
     <t>14</t>
   </si>
   <si>
-    <t>W2305300410-01</t>
-  </si>
-  <si>
-    <t>5B</t>
-  </si>
-  <si>
-    <t>9</t>
+    <t>20A</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>AE</t>
+  </si>
+  <si>
+    <t>40B</t>
+  </si>
+  <si>
+    <t>37B</t>
+  </si>
+  <si>
+    <t>41</t>
+  </si>
+  <si>
+    <t>2309193276</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>AD</t>
+  </si>
+  <si>
+    <t>19A</t>
+  </si>
+  <si>
+    <t>2309193279</t>
+  </si>
+  <si>
+    <t>29</t>
+  </si>
+  <si>
+    <t>35A</t>
   </si>
 </sst>
 </file>
@@ -153,7 +183,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -161,6 +191,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -184,8 +215,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E3934BF8-7079-9546-BE9B-ED542DA726BE}" name="Table1" displayName="Table1" ref="A1:G14" totalsRowShown="0">
-  <autoFilter ref="A1:G14" xr:uid="{E3934BF8-7079-9546-BE9B-ED542DA726BE}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E3934BF8-7079-9546-BE9B-ED542DA726BE}" name="Table1" displayName="Table1" ref="A1:G42" totalsRowShown="0">
+  <autoFilter ref="A1:G42" xr:uid="{E3934BF8-7079-9546-BE9B-ED542DA726BE}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{080A13DC-68CA-5245-8943-FDF1A014A6A7}" name="Item"/>
     <tableColumn id="2" xr3:uid="{E5BE8C13-A597-C246-BC4D-77EF9D6A8D67}" name="Lot in Legacy"/>
@@ -516,10 +547,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{590CF6CC-C7C3-1B41-8D52-80F1232A80D7}">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -558,112 +589,112 @@
       <c r="A2" t="s">
         <v>7</v>
       </c>
-      <c r="B2">
-        <v>2305300406</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="B2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="2">
-        <v>3</v>
+      <c r="E2" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="F2">
-        <v>82.11</v>
+        <v>16.73</v>
       </c>
       <c r="G2">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>7</v>
       </c>
-      <c r="B3">
-        <v>2305300406</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="B3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D3" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>10</v>
+      <c r="E3" s="3" t="s">
+        <v>11</v>
       </c>
       <c r="F3">
-        <v>71.569999999999993</v>
+        <v>59.55</v>
       </c>
       <c r="G3">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="B4">
-        <v>2305300405</v>
-      </c>
-      <c r="C4" t="s">
-        <v>11</v>
+      <c r="B4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="D4" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="3" t="s">
         <v>12</v>
       </c>
       <c r="F4">
-        <v>12.22</v>
+        <v>50.84</v>
       </c>
       <c r="G4">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>7</v>
       </c>
-      <c r="B5">
-        <v>2305300405</v>
-      </c>
-      <c r="C5" t="s">
-        <v>11</v>
+      <c r="B5" s="2">
+        <v>2309151207</v>
+      </c>
+      <c r="C5" s="2">
+        <v>2309151207</v>
       </c>
       <c r="D5" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="3" t="s">
         <v>13</v>
       </c>
       <c r="F5">
-        <v>84.16</v>
+        <v>51.08</v>
       </c>
       <c r="G5">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>7</v>
       </c>
-      <c r="B6">
-        <v>2305300410</v>
-      </c>
-      <c r="C6" t="s">
-        <v>14</v>
+      <c r="B6" s="2">
+        <v>2309151207</v>
+      </c>
+      <c r="C6" s="2">
+        <v>2309151207</v>
       </c>
       <c r="D6" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>15</v>
+      <c r="E6" s="3" t="s">
+        <v>14</v>
       </c>
       <c r="F6">
-        <v>12.6</v>
+        <v>29.6</v>
       </c>
       <c r="G6">
         <v>158</v>
@@ -673,45 +704,269 @@
       <c r="A7" t="s">
         <v>7</v>
       </c>
-      <c r="B7">
-        <v>2305300410</v>
-      </c>
-      <c r="C7" t="s">
-        <v>14</v>
+      <c r="B7" s="2">
+        <v>2309151207</v>
+      </c>
+      <c r="C7" s="2">
+        <v>2309151207</v>
       </c>
       <c r="D7" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7">
+        <v>61.42</v>
+      </c>
+      <c r="G7">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2">
+        <v>2309193275</v>
+      </c>
+      <c r="C8" s="2">
+        <v>2309193275</v>
+      </c>
+      <c r="D8" t="s">
         <v>16</v>
       </c>
-      <c r="F7">
-        <v>63.64</v>
-      </c>
-      <c r="G7">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="E8" s="1"/>
+      <c r="E8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8">
+        <v>2.4</v>
+      </c>
+      <c r="G8">
+        <v>157</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="E9" s="1"/>
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="2">
+        <v>2309193275</v>
+      </c>
+      <c r="C9" s="2">
+        <v>2309193275</v>
+      </c>
+      <c r="D9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9">
+        <v>35.32</v>
+      </c>
+      <c r="G9">
+        <v>157</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="E10" s="1"/>
+      <c r="A10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="2">
+        <v>2309193275</v>
+      </c>
+      <c r="C10" s="2">
+        <v>2309193275</v>
+      </c>
+      <c r="D10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F10">
+        <v>64.069999999999993</v>
+      </c>
+      <c r="G10">
+        <v>157</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="E11" s="1"/>
+      <c r="A11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F11">
+        <v>66.349999999999994</v>
+      </c>
+      <c r="G11">
+        <v>157</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="E12" s="1"/>
+      <c r="A12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F12">
+        <v>56.43</v>
+      </c>
+      <c r="G12">
+        <v>155</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="E13" s="1"/>
+      <c r="A13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F13">
+        <v>65</v>
+      </c>
+      <c r="G13">
+        <v>157</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="E14" s="1"/>
+      <c r="A14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" t="s">
+        <v>22</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F14">
+        <v>39.5</v>
+      </c>
+      <c r="G14">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E15" s="3"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E16" s="3"/>
+    </row>
+    <row r="17" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E17" s="3"/>
+    </row>
+    <row r="18" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E18" s="3"/>
+    </row>
+    <row r="19" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E19" s="3"/>
+    </row>
+    <row r="20" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E20" s="3"/>
+    </row>
+    <row r="21" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E21" s="3"/>
+    </row>
+    <row r="22" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E22" s="3"/>
+    </row>
+    <row r="23" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E23" s="3"/>
+    </row>
+    <row r="24" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E24" s="3"/>
+    </row>
+    <row r="25" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E25" s="3"/>
+    </row>
+    <row r="26" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E26" s="3"/>
+    </row>
+    <row r="27" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E27" s="3"/>
+    </row>
+    <row r="28" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E28"/>
+    </row>
+    <row r="29" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E29" s="3"/>
+    </row>
+    <row r="30" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E30" s="3"/>
+    </row>
+    <row r="31" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E31" s="3"/>
+    </row>
+    <row r="32" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E32" s="3"/>
+    </row>
+    <row r="33" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E33" s="3"/>
+    </row>
+    <row r="34" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E34" s="3"/>
+    </row>
+    <row r="35" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E35" s="3"/>
+    </row>
+    <row r="36" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E36" s="3"/>
+    </row>
+    <row r="37" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E37" s="3"/>
+    </row>
+    <row r="38" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E38" s="3"/>
+    </row>
+    <row r="39" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E39" s="3"/>
+    </row>
+    <row r="40" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E40" s="3"/>
+    </row>
+    <row r="41" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E41" s="3"/>
+    </row>
+    <row r="42" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E42" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>